<commit_message>
Funcionalidad reporte plano para un organigrama finalizado
</commit_message>
<xml_diff>
--- a/src/main/resources/reports/organizationChart/organizationChart.xlsx
+++ b/src/main/resources/reports/organizationChart/organizationChart.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\PROYECTOS\FORTELECIMEITO Y MODERNIZACION INSTITUCIONAL\APP\Carga-Trabajo-Services\src\main\resources\reports\organizationChart\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10E6026C-0289-4022-B423-BDDAD2F77180}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E15A0BC-8B62-4316-8B84-20AE33FC188F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{FC55D6EF-68F2-426F-9839-57243A004983}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{FC55D6EF-68F2-426F-9839-57243A004983}"/>
   </bookViews>
   <sheets>
     <sheet name="Detalle por dependencia" sheetId="2" r:id="rId1"/>
@@ -61,7 +61,7 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-jx:area(lastCell="M12");
+jx:area(lastCell="M14");
 jx:image(src="logo" lastCell="B3" imageType="PNG");</t>
         </r>
       </text>
@@ -74,7 +74,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Leonel Perez:</t>
         </r>
@@ -83,7 +83,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 jx:mergeCells(cols="size(levels) + 10" rows="1" minCols="1" minRows="1" lastCell="C2");</t>
@@ -98,7 +98,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Leonel Perez:</t>
         </r>
@@ -107,7 +107,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 jx:mergeCells(cols="size(levels) + 10" rows="1" minCols="1" minRows="1" lastCell="C3");</t>
@@ -122,7 +122,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Leonel Perez:</t>
         </r>
@@ -131,22 +131,22 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 jx:mergeCells(cols="size(levels) + 11" rows="1" minCols="1" minRows="1" lastCell="B5");</t>
         </r>
       </text>
     </comment>
-    <comment ref="M7" authorId="1" shapeId="0" xr:uid="{3512C239-376A-49EC-A072-AC72A15ABACC}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
+    <comment ref="B7" authorId="1" shapeId="0" xr:uid="{74EB7866-986B-42AB-AA37-72E36DD10FD5}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>Leonel Perez:</t>
         </r>
@@ -155,22 +155,22 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-jx:merge(cols="size(levels)" rows="1" minCols="1" minRows="1" lastCell="M7");</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="M8" authorId="1" shapeId="0" xr:uid="{2B3699D8-7DBA-4BDF-B53A-C9DF7B10AA5E}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+jx:mergeCells(cols="size(levels)+11" rows="1" minCols="1" minRows="1" lastCell="B7");</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B8" authorId="1" shapeId="0" xr:uid="{F59D9867-4595-4C6C-8F55-041A59FF0AFD}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>Leonel Perez:</t>
         </r>
@@ -179,22 +179,22 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-jx:each(items="levels" var="level" lastCell="M8" direction="RIGHT");</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B9" authorId="1" shapeId="0" xr:uid="{E2FF3263-85AD-4C16-9B8D-D8F2E00C85FD}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+jx:mergeCells(cols="size(levels)+11" rows="1" minCols="1" minRows="1" lastCell="B8");</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M10" authorId="1" shapeId="0" xr:uid="{3512C239-376A-49EC-A072-AC72A15ABACC}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>Leonel Perez:</t>
         </r>
@@ -203,22 +203,70 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-jx:each(items="dataOperationalManagement" var="reporte" lastCell="M9");</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="M9" authorId="1" shapeId="0" xr:uid="{3CF41AF4-6086-4D16-B3E0-F2EE151FABA3}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+jx:merge(cols="size(levels)" rows="1" minCols="1" minRows="1" lastCell="M10");</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M11" authorId="1" shapeId="0" xr:uid="{2B3699D8-7DBA-4BDF-B53A-C9DF7B10AA5E}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Leonel Perez:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+jx:each(items="levels" var="level" lastCell="M11" direction="RIGHT");</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B12" authorId="1" shapeId="0" xr:uid="{E2FF3263-85AD-4C16-9B8D-D8F2E00C85FD}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Leonel Perez:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+jx:each(items="dataOperationalManagement" var="reporte" lastCell="M12");</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M12" authorId="1" shapeId="0" xr:uid="{3CF41AF4-6086-4D16-B3E0-F2EE151FABA3}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>USER:</t>
         </r>
@@ -227,22 +275,22 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-jx:each(items="reporte.tiemposPorNivel" var="time" lastCell="M9" direction="RIGHT");</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="M10" authorId="1" shapeId="0" xr:uid="{0D372A5D-10DA-4BAF-BFA2-50705B7E88B7}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+jx:each(items="reporte.tiemposPorNivel" var="time" lastCell="M12" direction="RIGHT");</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M13" authorId="1" shapeId="0" xr:uid="{0D372A5D-10DA-4BAF-BFA2-50705B7E88B7}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>Leonel Perez:</t>
         </r>
@@ -251,22 +299,22 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-jx:each(items="T.sum('tiemposPorNivel', 'dataOperationalManagement', '')" var="time" lastCell="M10" direction="RIGHT");</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="M11" authorId="1" shapeId="0" xr:uid="{D4CA8420-816E-4B04-A490-50703CEBA954}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+jx:each(items="T.sum('tiemposPorNivel', 'dataOperationalManagement', '')" var="time" lastCell="M13" direction="RIGHT");</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M14" authorId="1" shapeId="0" xr:uid="{D4CA8420-816E-4B04-A490-50703CEBA954}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">Leonel Perez:
 </t>
@@ -276,9 +324,9 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>jx:each(items="T.sum('tiemposPorNivel', 'dataOperationalManagement', '')" var="time" lastCell="M11" direction="RIGHT");</t>
+            <family val="2"/>
+          </rPr>
+          <t>jx:each(items="T.sum('tiemposPorNivel', 'dataOperationalManagement', '')" var="time" lastCell="M14" direction="RIGHT");</t>
         </r>
       </text>
     </comment>
@@ -290,6 +338,7 @@
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Ronald Torres</author>
+    <author>USER</author>
   </authors>
   <commentList>
     <comment ref="B2" authorId="0" shapeId="0" xr:uid="{1111CF24-A031-4905-A36E-4EE1741775AA}">
@@ -312,7 +361,7 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-jx:area(lastCell="D10");
+jx:area(lastCell="D13");
 jx:image(src="logo" lastCell="B3" imageType="PNG");</t>
         </r>
       </text>
@@ -389,7 +438,55 @@
         </r>
       </text>
     </comment>
-    <comment ref="C7" authorId="0" shapeId="0" xr:uid="{003027D8-7366-4DB5-9DE6-671B22019C17}">
+    <comment ref="B7" authorId="1" shapeId="0" xr:uid="{38B29B99-8FA4-40EE-ACF3-B514BD16A860}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>USER:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+jx:mergeCells(cols="size(levels)+2" rows="1" minCols="1" minRows="1" lastCell="B7");</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B8" authorId="1" shapeId="0" xr:uid="{239F0718-9321-4D54-AB6F-9A09746D034F}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>USER:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+jx:mergeCells(cols="size(levels)+2" rows="1" minCols="1" minRows="1" lastCell="B8");</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C10" authorId="0" shapeId="0" xr:uid="{003027D8-7366-4DB5-9DE6-671B22019C17}">
       <text>
         <r>
           <rPr>
@@ -409,11 +506,11 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-jx:merge(cols="size(levels)" rows="1" minCols="1" minRows="1" lastCell="C7");</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="C8" authorId="0" shapeId="0" xr:uid="{BE1D5D99-EBE2-4B60-9D12-B22D3F2F9180}">
+jx:merge(cols="size(levels)" rows="1" minCols="1" minRows="1" lastCell="C10");</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C11" authorId="0" shapeId="0" xr:uid="{BE1D5D99-EBE2-4B60-9D12-B22D3F2F9180}">
       <text>
         <r>
           <rPr>
@@ -433,11 +530,11 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-jx:each(items="levels" var="level" lastCell="C8" direction="RIGHT");</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B9" authorId="0" shapeId="0" xr:uid="{762C841B-2997-4098-B8E5-179A533F5391}">
+jx:each(items="levels" var="level" lastCell="C11" direction="RIGHT");</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B12" authorId="0" shapeId="0" xr:uid="{762C841B-2997-4098-B8E5-179A533F5391}">
       <text>
         <r>
           <rPr>
@@ -457,11 +554,11 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-jx:each(items="plainProcess" var="resultado" lastCell="D9");</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="C9" authorId="0" shapeId="0" xr:uid="{3A29FB23-0221-4817-82D9-3B600EEF5FF7}">
+jx:each(items="plainProcess" var="resultado" lastCell="D12");</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C12" authorId="0" shapeId="0" xr:uid="{3A29FB23-0221-4817-82D9-3B600EEF5FF7}">
       <text>
         <r>
           <rPr>
@@ -481,11 +578,11 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-jx:each(items="resultado.tiemposPorNivel" var="time" lastCell="C9" direction="RIGHT");</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="C10" authorId="0" shapeId="0" xr:uid="{E4542BDC-78B4-472A-94D9-4ACC2A76EF5C}">
+jx:each(items="resultado.tiemposPorNivel" var="time" lastCell="C12" direction="RIGHT");</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C13" authorId="0" shapeId="0" xr:uid="{E4542BDC-78B4-472A-94D9-4ACC2A76EF5C}">
       <text>
         <r>
           <rPr>
@@ -505,7 +602,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>jx:each(items="levels" var="level" lastCell="C10" direction="RIGHT");
+          <t>jx:each(items="levels" var="level" lastCell="C13" direction="RIGHT");
 jx:params(formulaStrategy="BY_COLUMN")</t>
         </r>
       </text>
@@ -515,7 +612,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="41">
   <si>
     <t>Gestión y Desarrollo del Talento Humano</t>
   </si>
@@ -553,9 +650,6 @@
     <t>DEPENDENCIA</t>
   </si>
   <si>
-    <t>$[SUM(C9)]</t>
-  </si>
-  <si>
     <t xml:space="preserve">TOTAL DE EMPLEOS </t>
   </si>
   <si>
@@ -565,9 +659,6 @@
     <t>NÚMERO DE EMPLEOS DISTRIBUIDOS POR NIVELES Y DENOMINACIONES DE EMPLEOS</t>
   </si>
   <si>
-    <t>$[SUM(C10)]</t>
-  </si>
-  <si>
     <t>NOMENCLATURA DEL NIVEL</t>
   </si>
   <si>
@@ -629,6 +720,21 @@
   </si>
   <si>
     <t>Gestión de Tiempos Laborados por Proceso</t>
+  </si>
+  <si>
+    <t>${organizationChart.nombre}</t>
+  </si>
+  <si>
+    <t>${organizationChart.descripcion}</t>
+  </si>
+  <si>
+    <t>$[SUMIF(C12, "&gt;0")]</t>
+  </si>
+  <si>
+    <t>$[SUMIF(C13, "&gt;0")]</t>
+  </si>
+  <si>
+    <t>$[SUM(C12)]</t>
   </si>
 </sst>
 </file>
@@ -757,17 +863,17 @@
       <family val="1"/>
     </font>
     <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
-    </font>
-    <font>
       <b/>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Georgia Pro Black"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Georgia Pro Black"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="6">
@@ -940,7 +1046,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1009,6 +1115,18 @@
     </xf>
     <xf numFmtId="2" fontId="7" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -1389,10 +1507,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{893D9117-F19F-4DD0-B7E0-678E6E9A8AE8}">
-  <dimension ref="B1:U22"/>
+  <dimension ref="B1:U25"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="L9" sqref="L9"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.375" defaultRowHeight="15.75"/>
@@ -1408,16 +1526,16 @@
   <sheetData>
     <row r="1" spans="2:21" ht="16.5" thickBot="1"/>
     <row r="2" spans="2:21" s="10" customFormat="1" ht="30" customHeight="1">
-      <c r="B2" s="36"/>
+      <c r="B2" s="40"/>
       <c r="C2" s="3" t="s">
         <v>0</v>
       </c>
       <c r="M2" s="24"/>
     </row>
     <row r="3" spans="2:21" s="9" customFormat="1" ht="30" customHeight="1" thickBot="1">
-      <c r="B3" s="37"/>
+      <c r="B3" s="41"/>
       <c r="C3" s="17" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="H3" s="21"/>
       <c r="I3" s="21"/>
@@ -1430,170 +1548,201 @@
       </c>
     </row>
     <row r="6" spans="2:21" s="5" customFormat="1"/>
-    <row r="7" spans="2:21" s="6" customFormat="1" ht="20.100000000000001" customHeight="1">
-      <c r="B7" s="34" t="s">
+    <row r="7" spans="2:21" s="5" customFormat="1" ht="30" customHeight="1">
+      <c r="B7" s="29" t="s">
+        <v>36</v>
+      </c>
+      <c r="C7" s="27"/>
+      <c r="D7" s="27"/>
+      <c r="E7" s="27"/>
+      <c r="F7" s="27"/>
+      <c r="G7" s="27"/>
+      <c r="H7" s="27"/>
+      <c r="I7" s="27"/>
+      <c r="J7" s="27"/>
+      <c r="K7" s="27"/>
+      <c r="L7" s="27"/>
+    </row>
+    <row r="8" spans="2:21" s="5" customFormat="1" ht="30" customHeight="1">
+      <c r="B8" s="30" t="s">
+        <v>37</v>
+      </c>
+      <c r="C8" s="28"/>
+      <c r="D8" s="28"/>
+      <c r="E8" s="28"/>
+      <c r="F8" s="28"/>
+      <c r="G8" s="28"/>
+      <c r="H8" s="28"/>
+      <c r="I8" s="28"/>
+      <c r="J8" s="28"/>
+      <c r="K8" s="28"/>
+      <c r="L8" s="28"/>
+    </row>
+    <row r="9" spans="2:21" s="5" customFormat="1"/>
+    <row r="10" spans="2:21" s="6" customFormat="1" ht="20.100000000000001" customHeight="1">
+      <c r="B10" s="38" t="s">
+        <v>17</v>
+      </c>
+      <c r="C10" s="38" t="s">
+        <v>18</v>
+      </c>
+      <c r="D10" s="38" t="s">
+        <v>16</v>
+      </c>
+      <c r="E10" s="38" t="s">
+        <v>11</v>
+      </c>
+      <c r="F10" s="38" t="s">
+        <v>1</v>
+      </c>
+      <c r="G10" s="37" t="s">
+        <v>15</v>
+      </c>
+      <c r="H10" s="42" t="s">
+        <v>2</v>
+      </c>
+      <c r="I10" s="42" t="s">
+        <v>3</v>
+      </c>
+      <c r="J10" s="42" t="s">
+        <v>4</v>
+      </c>
+      <c r="K10" s="42" t="s">
+        <v>5</v>
+      </c>
+      <c r="L10" s="42" t="s">
+        <v>7</v>
+      </c>
+      <c r="M10" s="23" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="2:21" s="6" customFormat="1" ht="20.100000000000001" customHeight="1">
+      <c r="B11" s="39"/>
+      <c r="C11" s="39"/>
+      <c r="D11" s="39"/>
+      <c r="E11" s="39"/>
+      <c r="F11" s="39"/>
+      <c r="G11" s="37"/>
+      <c r="H11" s="42"/>
+      <c r="I11" s="42"/>
+      <c r="J11" s="42"/>
+      <c r="K11" s="42"/>
+      <c r="L11" s="42"/>
+      <c r="M11" s="23" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="12" spans="2:21" s="5" customFormat="1" ht="15" customHeight="1">
+      <c r="B12" s="22" t="s">
+        <v>20</v>
+      </c>
+      <c r="C12" s="22" t="s">
+        <v>21</v>
+      </c>
+      <c r="D12" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="E12" s="22" t="s">
+        <v>23</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="H12" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="I12" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="J12" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="K12" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="L12" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="M12" s="14" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="13" spans="2:21" s="11" customFormat="1" ht="18" customHeight="1">
+      <c r="B13" s="34" t="s">
         <v>19</v>
       </c>
-      <c r="C7" s="34" t="s">
-        <v>20</v>
-      </c>
-      <c r="D7" s="34" t="s">
-        <v>18</v>
-      </c>
-      <c r="E7" s="34" t="s">
-        <v>11</v>
-      </c>
-      <c r="F7" s="34" t="s">
-        <v>1</v>
-      </c>
-      <c r="G7" s="33" t="s">
-        <v>17</v>
-      </c>
-      <c r="H7" s="38" t="s">
-        <v>2</v>
-      </c>
-      <c r="I7" s="38" t="s">
-        <v>3</v>
-      </c>
-      <c r="J7" s="38" t="s">
-        <v>4</v>
-      </c>
-      <c r="K7" s="38" t="s">
-        <v>5</v>
-      </c>
-      <c r="L7" s="38" t="s">
-        <v>7</v>
-      </c>
-      <c r="M7" s="23" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="2:21" s="6" customFormat="1" ht="20.100000000000001" customHeight="1">
-      <c r="B8" s="35"/>
-      <c r="C8" s="35"/>
-      <c r="D8" s="35"/>
-      <c r="E8" s="35"/>
-      <c r="F8" s="35"/>
-      <c r="G8" s="33"/>
-      <c r="H8" s="38"/>
-      <c r="I8" s="38"/>
-      <c r="J8" s="38"/>
-      <c r="K8" s="38"/>
-      <c r="L8" s="38"/>
-      <c r="M8" s="23" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="9" spans="2:21" s="5" customFormat="1" ht="15" customHeight="1">
-      <c r="B9" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="C9" s="22" t="s">
-        <v>23</v>
-      </c>
-      <c r="D9" s="22" t="s">
-        <v>24</v>
-      </c>
-      <c r="E9" s="22" t="s">
-        <v>25</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="G9" s="2" t="s">
+      <c r="C13" s="35"/>
+      <c r="D13" s="35"/>
+      <c r="E13" s="35"/>
+      <c r="F13" s="36"/>
+      <c r="G13" s="18"/>
+      <c r="H13" s="18"/>
+      <c r="I13" s="18"/>
+      <c r="J13" s="18"/>
+      <c r="K13" s="18"/>
+      <c r="L13" s="18"/>
+      <c r="M13" s="26" t="s">
         <v>33</v>
       </c>
-      <c r="H9" s="14" t="s">
-        <v>27</v>
-      </c>
-      <c r="I9" s="14" t="s">
-        <v>28</v>
-      </c>
-      <c r="J9" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="K9" s="14" t="s">
-        <v>30</v>
-      </c>
-      <c r="L9" s="14" t="s">
-        <v>31</v>
-      </c>
-      <c r="M9" s="14" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="10" spans="2:21" s="11" customFormat="1" ht="18" customHeight="1">
-      <c r="B10" s="30" t="s">
-        <v>21</v>
-      </c>
-      <c r="C10" s="31"/>
-      <c r="D10" s="31"/>
-      <c r="E10" s="31"/>
-      <c r="F10" s="32"/>
-      <c r="G10" s="18"/>
-      <c r="H10" s="18"/>
-      <c r="I10" s="18"/>
-      <c r="J10" s="18"/>
-      <c r="K10" s="18"/>
-      <c r="L10" s="18"/>
-      <c r="M10" s="26" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="11" spans="2:21" s="5" customFormat="1" ht="30" customHeight="1">
-      <c r="B11" s="27" t="s">
+    </row>
+    <row r="14" spans="2:21" s="5" customFormat="1" ht="30" customHeight="1">
+      <c r="B14" s="31" t="s">
         <v>9</v>
       </c>
-      <c r="C11" s="28"/>
-      <c r="D11" s="28"/>
-      <c r="E11" s="28"/>
-      <c r="F11" s="29"/>
-      <c r="G11" s="13"/>
-      <c r="H11" s="13"/>
-      <c r="I11" s="13"/>
-      <c r="J11" s="13"/>
-      <c r="K11" s="13"/>
-      <c r="L11" s="13"/>
-      <c r="M11" s="15" t="s">
+      <c r="C14" s="32"/>
+      <c r="D14" s="32"/>
+      <c r="E14" s="32"/>
+      <c r="F14" s="33"/>
+      <c r="G14" s="13"/>
+      <c r="H14" s="13"/>
+      <c r="I14" s="13"/>
+      <c r="J14" s="13"/>
+      <c r="K14" s="13"/>
+      <c r="L14" s="13"/>
+      <c r="M14" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="U11" s="20"/>
-    </row>
-    <row r="12" spans="2:21" s="5" customFormat="1"/>
-    <row r="13" spans="2:21" s="5" customFormat="1"/>
-    <row r="14" spans="2:21" s="5" customFormat="1"/>
+      <c r="U14" s="20"/>
+    </row>
     <row r="15" spans="2:21" s="5" customFormat="1"/>
     <row r="16" spans="2:21" s="5" customFormat="1"/>
     <row r="17" spans="3:18" s="5" customFormat="1"/>
-    <row r="18" spans="3:18" s="5" customFormat="1">
-      <c r="C18" s="20"/>
-    </row>
-    <row r="20" spans="3:18">
-      <c r="G20" s="19"/>
-    </row>
-    <row r="21" spans="3:18">
-      <c r="C21" s="19"/>
-    </row>
-    <row r="22" spans="3:18">
-      <c r="I22" s="19"/>
-      <c r="R22" s="19"/>
+    <row r="18" spans="3:18" s="5" customFormat="1"/>
+    <row r="19" spans="3:18" s="5" customFormat="1"/>
+    <row r="20" spans="3:18" s="5" customFormat="1"/>
+    <row r="21" spans="3:18" s="5" customFormat="1">
+      <c r="C21" s="20"/>
+    </row>
+    <row r="23" spans="3:18">
+      <c r="G23" s="19"/>
+    </row>
+    <row r="24" spans="3:18">
+      <c r="C24" s="19"/>
+    </row>
+    <row r="25" spans="3:18">
+      <c r="I25" s="19"/>
+      <c r="R25" s="19"/>
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="L7:L8"/>
-    <mergeCell ref="I7:I8"/>
-    <mergeCell ref="J7:J8"/>
-    <mergeCell ref="K7:K8"/>
-    <mergeCell ref="H7:H8"/>
-    <mergeCell ref="B11:F11"/>
-    <mergeCell ref="B10:F10"/>
-    <mergeCell ref="G7:G8"/>
-    <mergeCell ref="F7:F8"/>
+    <mergeCell ref="L10:L11"/>
+    <mergeCell ref="I10:I11"/>
+    <mergeCell ref="J10:J11"/>
+    <mergeCell ref="K10:K11"/>
+    <mergeCell ref="H10:H11"/>
+    <mergeCell ref="B14:F14"/>
+    <mergeCell ref="B13:F13"/>
+    <mergeCell ref="G10:G11"/>
+    <mergeCell ref="F10:F11"/>
     <mergeCell ref="B2:B3"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="D7:D8"/>
-    <mergeCell ref="C7:C8"/>
-    <mergeCell ref="E7:E8"/>
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="D10:D11"/>
+    <mergeCell ref="C10:C11"/>
+    <mergeCell ref="E10:E11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1603,10 +1752,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1120979F-9C31-4613-A024-CA2A89E9F169}">
-  <dimension ref="B1:D17"/>
+  <dimension ref="B1:D20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.375" defaultRowHeight="15.75"/>
@@ -1620,15 +1769,15 @@
   <sheetData>
     <row r="1" spans="2:4" ht="16.5" thickBot="1"/>
     <row r="2" spans="2:4" s="10" customFormat="1" ht="30" customHeight="1">
-      <c r="B2" s="36"/>
+      <c r="B2" s="40"/>
       <c r="C2" s="3" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="3" spans="2:4" s="9" customFormat="1" ht="30" customHeight="1" thickBot="1">
-      <c r="B3" s="37"/>
+      <c r="B3" s="41"/>
       <c r="C3" s="4" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="4" spans="2:4" s="5" customFormat="1"/>
@@ -1638,58 +1787,69 @@
       </c>
     </row>
     <row r="6" spans="2:4" s="5" customFormat="1"/>
-    <row r="7" spans="2:4" s="6" customFormat="1" ht="20.100000000000001" customHeight="1">
-      <c r="B7" s="34" t="s">
-        <v>19</v>
-      </c>
-      <c r="C7" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="D7" s="38" t="s">
+    <row r="7" spans="2:4" s="5" customFormat="1" ht="30" customHeight="1">
+      <c r="B7" s="29" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="8" spans="2:4" s="5" customFormat="1" ht="30" customHeight="1">
+      <c r="B8" s="30" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="9" spans="2:4" s="5" customFormat="1"/>
+    <row r="10" spans="2:4" s="6" customFormat="1" ht="20.100000000000001" customHeight="1">
+      <c r="B10" s="38" t="s">
+        <v>17</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D10" s="42" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="2:4" s="6" customFormat="1" ht="20.100000000000001" customHeight="1">
+      <c r="B11" s="39"/>
+      <c r="C11" s="7" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="8" spans="2:4" s="6" customFormat="1" ht="20.100000000000001" customHeight="1">
-      <c r="B8" s="35"/>
-      <c r="C8" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="D8" s="38"/>
-    </row>
-    <row r="9" spans="2:4" s="5" customFormat="1" ht="15" customHeight="1">
-      <c r="B9" s="12" t="s">
-        <v>36</v>
-      </c>
-      <c r="C9" s="14" t="s">
+      <c r="D11" s="42"/>
+    </row>
+    <row r="12" spans="2:4" s="5" customFormat="1" ht="15" customHeight="1">
+      <c r="B12" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="C12" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="D9" s="14" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="10" spans="2:4" s="5" customFormat="1" ht="30" customHeight="1">
-      <c r="B10" s="13" t="s">
+      <c r="D12" s="14" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="13" spans="2:4" s="5" customFormat="1" ht="30" customHeight="1">
+      <c r="B13" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="C10" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="D10" s="15" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="11" spans="2:4" s="5" customFormat="1"/>
-    <row r="12" spans="2:4" s="5" customFormat="1"/>
-    <row r="13" spans="2:4" s="5" customFormat="1"/>
+      <c r="C13" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="D13" s="15" t="s">
+        <v>39</v>
+      </c>
+    </row>
     <row r="14" spans="2:4" s="5" customFormat="1"/>
     <row r="15" spans="2:4" s="5" customFormat="1"/>
     <row r="16" spans="2:4" s="5" customFormat="1"/>
     <row r="17" s="5" customFormat="1"/>
+    <row r="18" s="5" customFormat="1"/>
+    <row r="19" s="5" customFormat="1"/>
+    <row r="20" s="5" customFormat="1"/>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="B10:B11"/>
     <mergeCell ref="B2:B3"/>
-    <mergeCell ref="D7:D8"/>
+    <mergeCell ref="D10:D11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>

</xml_diff>